<commit_message>
vault backup: 2024-08-09 16:43:03 3
</commit_message>
<xml_diff>
--- a/Year 1 - Sem 1/ITC 1370 - IT/ITC - Activities/Activity 01-20240808/01 SS-Activities for students.xlsx
+++ b/Year 1 - Sem 1/ITC 1370 - IT/ITC - Activities/Activity 01-20240808/01 SS-Activities for students.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\REDTECH\OneDrive\Documents\Obsidian\USJ-BMC\Year 1 - Sem 1\ITC 1370 - IT\ITC - Activities\Activity 01-20240808\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1BD1E2-C851-49BE-B07B-C3C60038F921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity 01.1" sheetId="1" r:id="rId1"/>
@@ -335,17 +341,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$Rs.-849]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$Rs.-849]\ #,##0.0"/>
     <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -491,47 +504,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -539,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -553,6 +557,23 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
@@ -768,7 +789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1798,16 +1819,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A3" sqref="A3:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="5" width="12.85546875" customWidth="1"/>
@@ -1825,6 +1846,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1833,14 +1857,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
       <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+    </row>
     <row r="6" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="23"/>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -1864,6 +1890,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1878,6 +1905,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1892,6 +1920,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
       <c r="C9" t="s">
         <v>21</v>
       </c>
@@ -1903,6 +1932,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -2907,17 +2937,20 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H6" sqref="H6:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,39 +2963,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2988,7 +3021,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="7">
         <v>44932</v>
       </c>
@@ -3012,7 +3045,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="7">
         <v>44949</v>
       </c>
@@ -3036,7 +3069,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="7">
         <v>44966</v>
       </c>
@@ -3060,7 +3093,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="7">
         <v>44983</v>
       </c>
@@ -3084,7 +3117,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="7">
         <v>45000</v>
       </c>
@@ -3108,7 +3141,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="7">
         <v>45017</v>
       </c>
@@ -3132,7 +3165,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="7">
         <v>45034</v>
       </c>
@@ -3156,7 +3189,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="7">
         <v>45051</v>
       </c>
@@ -3180,7 +3213,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="7">
         <v>45068</v>
       </c>
@@ -3204,7 +3237,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="7">
         <v>45085</v>
       </c>
@@ -3228,7 +3261,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="7">
         <v>45102</v>
       </c>
@@ -3252,7 +3285,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="13"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="7">
         <v>45119</v>
       </c>
@@ -3280,12 +3313,21 @@
     <mergeCell ref="B2:I4"/>
     <mergeCell ref="B5:B17"/>
   </mergeCells>
+  <conditionalFormatting sqref="H6:H17">
+    <cfRule type="iconSet" priority="1">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CW1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15011,7 +15053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16147,17 +16189,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -16166,34 +16208,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" t="s">
         <v>76</v>
       </c>
@@ -16203,311 +16245,311 @@
       <c r="E3" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="17">
         <v>129139</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <v>307763</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="17">
         <v>319624</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>490622</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="17">
         <v>331262</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="17">
         <v>363120</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="17">
         <v>221149</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="17">
         <v>447173</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="17">
         <v>307616</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>439608</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <v>372911</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <v>458387</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="17">
         <v>356349</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>191726</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="17">
         <v>211993</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="17">
         <v>414083</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="17">
         <v>458828</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="17">
         <v>193911</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="17">
         <v>236733</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <v>426152</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="17">
         <v>286725</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>404189</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="17">
         <v>300688</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="17">
         <v>201997</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <v>358499</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <v>385759</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <v>210294</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="17">
         <v>393917</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="17">
         <v>280241.66666666698</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>137803</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="17">
         <v>322907</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="17">
         <v>156032</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="17">
         <v>474982</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="17">
         <v>439352</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="17">
         <v>420997</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="17">
         <v>361682</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="17">
         <v>257973.16666666701</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>489467</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="17">
         <v>103737</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="17">
         <v>408034</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="17">
         <v>335548</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <v>244815</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="17">
         <v>312221</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="17">
         <v>329447</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="17">
         <v>235704.66666666701</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>315517</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="17">
         <v>475654</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="17">
         <v>176199</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="17">
         <v>297038</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="17">
         <v>340236</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="17">
         <v>111074</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="17">
         <v>297212</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="17">
         <v>213436.16666666701</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>224907</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="17">
         <v>141318</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="17">
         <v>278489</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="17">
         <v>416315</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="17">
         <v>174574</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="17">
         <v>199323</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="17">
         <v>264977</v>
       </c>
       <c r="G11">
         <v>191167.66666666701</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>446872</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="17">
         <v>462746</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="17">
         <v>411415</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="17">
         <v>131088</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <v>224298</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <v>492213</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <v>232742</v>
       </c>
       <c r="G12">
         <v>168899.16666666701</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>157388</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="17">
         <v>117652</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="17">
         <v>171955</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="17">
         <v>349688</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <v>150656</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <v>303700</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>200507</v>
       </c>
       <c r="G13">
         <v>146630.66666666701</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>100485</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="17">
         <v>300113</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="17">
         <v>424714</v>
       </c>
     </row>
@@ -16515,19 +16557,25 @@
       <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="16"/>
       <c r="K14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>